<commit_message>
The space after “Year” has been deleted.
</commit_message>
<xml_diff>
--- a/data/victoria_vehicle_registration_cleaned.xlsx
+++ b/data/victoria_vehicle_registration_cleaned.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Monash\Semester 4\FIT5120\Onboarding_Project\findmyspot\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhenhao Liu\Documents\Monash_University\FIT5120\Onboarding\Findmyspot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A79BC7B-CFC2-4535-A04C-F67D2D944506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557D9644-C898-402B-9607-504B3029599B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="27">
   <si>
     <t>Victoria</t>
   </si>
@@ -127,10 +127,6 @@
   </si>
   <si>
     <t>PASSENGER VEHICLES</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Year </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -142,20 +138,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -174,7 +170,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -216,7 +212,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -257,10 +253,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -268,8 +264,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币" xfId="1" builtinId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -550,31 +546,31 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.21875" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" customWidth="1"/>
+    <col min="1" max="1" width="30.25" customWidth="1"/>
+    <col min="2" max="2" width="11.25" customWidth="1"/>
+    <col min="3" max="3" width="11.58203125" customWidth="1"/>
+    <col min="4" max="4" width="11.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C1" s="18"/>
       <c r="D1" s="18"/>
       <c r="E1" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" s="15">
         <v>2016</v>
       </c>
@@ -585,7 +581,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -602,7 +598,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -619,7 +615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -636,7 +632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -653,7 +649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -670,7 +666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -687,7 +683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -704,7 +700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -721,7 +717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -738,7 +734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -775,17 +771,17 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="31.109375" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
-    <col min="6" max="6" width="30.109375" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="31.08203125" customWidth="1"/>
+    <col min="4" max="4" width="13.08203125" customWidth="1"/>
+    <col min="6" max="6" width="30.08203125" customWidth="1"/>
+    <col min="7" max="7" width="12.08203125" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>10</v>
       </c>
@@ -802,7 +798,7 @@
       <c r="H1" s="18"/>
       <c r="I1" s="18"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -821,7 +817,7 @@
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -839,7 +835,7 @@
       <c r="I3" s="17"/>
       <c r="J3" s="15"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
@@ -857,7 +853,7 @@
       <c r="I4" s="16"/>
       <c r="J4" s="15"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -875,7 +871,7 @@
       <c r="I5" s="16"/>
       <c r="J5" s="15"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -893,7 +889,7 @@
       <c r="I6" s="16"/>
       <c r="J6" s="15"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>0</v>
       </c>
@@ -911,7 +907,7 @@
       <c r="I7" s="16"/>
       <c r="J7" s="15"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -929,7 +925,7 @@
       <c r="I8" s="16"/>
       <c r="J8" s="15"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -947,7 +943,7 @@
       <c r="I9" s="16"/>
       <c r="J9" s="15"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>0</v>
       </c>
@@ -965,7 +961,7 @@
       <c r="I10" s="16"/>
       <c r="J10" s="15"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>9</v>
       </c>
@@ -983,7 +979,7 @@
       <c r="I11" s="16"/>
       <c r="J11" s="15"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1001,7 +997,7 @@
       <c r="I12" s="16"/>
       <c r="J12" s="15"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>0</v>
       </c>
@@ -1015,7 +1011,7 @@
         <v>43883</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>0</v>
       </c>
@@ -1029,7 +1025,7 @@
         <v>79506</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1043,7 +1039,7 @@
         <v>88175</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>0</v>
       </c>
@@ -1057,7 +1053,7 @@
         <v>89747</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>0</v>
       </c>
@@ -1071,7 +1067,7 @@
         <v>26779</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1085,7 +1081,7 @@
         <v>30010</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>0</v>
       </c>
@@ -1099,7 +1095,7 @@
         <v>31254</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>0</v>
       </c>
@@ -1113,7 +1109,7 @@
         <v>6550</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1127,7 +1123,7 @@
         <v>7466</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>0</v>
       </c>
@@ -1141,7 +1137,7 @@
         <v>7734</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>0</v>
       </c>
@@ -1155,7 +1151,7 @@
         <v>20302</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1169,7 +1165,7 @@
         <v>21853</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>0</v>
       </c>
@@ -1183,7 +1179,7 @@
         <v>20849</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>0</v>
       </c>
@@ -1197,7 +1193,7 @@
         <v>185248</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -1211,7 +1207,7 @@
         <v>198151</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>0</v>
       </c>
@@ -1225,7 +1221,7 @@
         <v>203317</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1239,7 +1235,7 @@
         <v>4681337</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -1253,7 +1249,7 @@
         <v>5119560</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>0</v>
       </c>

</xml_diff>